<commit_message>
Added stub for AI extension; see #126
- CSV for AI
- path: /ai for extension
- namespace: ai
- contains RDF and HTML stubs
</commit_message>
<xml_diff>
--- a/code/vocab_csv/process.xlsx
+++ b/code/vocab_csv/process.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="298">
   <si>
     <t>preffix</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Justifications for use with DPV concepts</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/ai#</t>
+  </si>
+  <si>
+    <t>AI Technology concepts extending DPV</t>
   </si>
   <si>
     <t>dct</t>
@@ -1956,6 +1965,20 @@
         <v>11</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -1982,8 +2005,9 @@
     <hyperlink r:id="rId22" ref="B21"/>
     <hyperlink r:id="rId23" ref="B22"/>
     <hyperlink r:id="rId24" ref="B23"/>
+    <hyperlink r:id="rId25" ref="B24"/>
   </hyperlinks>
-  <drawing r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -2029,13 +2053,13 @@
     </row>
     <row r="2">
       <c r="A2" s="19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -2059,13 +2083,13 @@
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
@@ -2089,13 +2113,13 @@
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
@@ -2119,13 +2143,13 @@
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -2149,13 +2173,13 @@
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
@@ -2179,13 +2203,13 @@
     </row>
     <row r="7">
       <c r="A7" s="19" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -2209,10 +2233,10 @@
     </row>
     <row r="8">
       <c r="A8" s="19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C8" s="25" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -2240,13 +2264,13 @@
     </row>
     <row r="9">
       <c r="A9" s="19" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -2270,13 +2294,13 @@
     </row>
     <row r="10">
       <c r="A10" s="19" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
@@ -2300,13 +2324,13 @@
     </row>
     <row r="11">
       <c r="A11" s="27" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
@@ -2330,13 +2354,13 @@
     </row>
     <row r="12">
       <c r="A12" s="19" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
@@ -2360,13 +2384,13 @@
     </row>
     <row r="13">
       <c r="A13" s="19" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -2390,13 +2414,13 @@
     </row>
     <row r="14">
       <c r="A14" s="27" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -2420,112 +2444,112 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2570,10 +2594,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="28" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>28</v>
@@ -2590,13 +2614,13 @@
     </row>
     <row r="2">
       <c r="A2" s="30" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -2610,13 +2634,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -2630,13 +2654,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -2645,18 +2669,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -2665,34 +2689,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -2706,13 +2730,13 @@
     </row>
     <row r="8">
       <c r="A8" s="30" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -2726,13 +2750,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -2746,13 +2770,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -2761,18 +2785,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -2781,18 +2805,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -2801,18 +2825,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -2826,13 +2850,13 @@
     </row>
     <row r="14">
       <c r="A14" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -2846,13 +2870,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -2866,13 +2890,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -2881,18 +2905,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -2901,18 +2925,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -2921,18 +2945,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -2946,13 +2970,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -2966,13 +2990,13 @@
     </row>
     <row r="21">
       <c r="A21" s="31" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D21" s="33">
         <v>44734.0</v>
@@ -3002,13 +3026,13 @@
     </row>
     <row r="22">
       <c r="A22" s="31" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D22" s="33">
         <v>44734.0</v>
@@ -3038,13 +3062,13 @@
     </row>
     <row r="23">
       <c r="A23" s="31" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D23" s="33">
         <v>44734.0</v>
@@ -3074,13 +3098,13 @@
     </row>
     <row r="24">
       <c r="A24" s="31" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D24" s="33">
         <v>45189.0</v>
@@ -3184,49 +3208,49 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="35" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -3246,25 +3270,25 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="8">
@@ -3274,30 +3298,30 @@
         <v>45270.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
@@ -3307,10 +3331,10 @@
       <c r="K3" s="41"/>
       <c r="L3" s="41"/>
       <c r="M3" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -3333,19 +3357,19 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
@@ -3355,10 +3379,10 @@
       <c r="K4" s="41"/>
       <c r="L4" s="41"/>
       <c r="M4" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
@@ -3381,34 +3405,34 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
       <c r="I5" s="6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
       <c r="M5" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
@@ -3431,60 +3455,60 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
       <c r="I7" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="J7" s="41"/>
       <c r="K7" s="41"/>
       <c r="L7" s="41"/>
       <c r="M7" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="41"/>
@@ -6450,49 +6474,49 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H1" s="47" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I1" s="47" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="J1" s="48" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="N1" s="50" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -6510,23 +6534,23 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E2" s="41" t="str">
         <f>CONCATENATE("dpv:",RIGHT(A2,LEN(A2) - 3))</f>
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -6537,13 +6561,13 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
@@ -6561,22 +6585,22 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>265</v>
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -6587,10 +6611,10 @@
       </c>
       <c r="L3" s="41"/>
       <c r="M3" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -6609,22 +6633,22 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
@@ -6635,10 +6659,10 @@
       </c>
       <c r="L4" s="41"/>
       <c r="M4" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
@@ -6657,22 +6681,22 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
@@ -6683,10 +6707,10 @@
       </c>
       <c r="L5" s="41"/>
       <c r="M5" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
@@ -6705,27 +6729,27 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
       <c r="I6" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="J6" s="41"/>
       <c r="K6" s="8">
@@ -6733,10 +6757,10 @@
       </c>
       <c r="L6" s="41"/>
       <c r="M6" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="41"/>
@@ -6755,22 +6779,22 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
@@ -6781,10 +6805,10 @@
       </c>
       <c r="L7" s="41"/>
       <c r="M7" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="41"/>
@@ -6824,43 +6848,43 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="C15" s="43"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C16" s="43"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C17" s="43"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C18" s="43"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C19" s="43"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C20" s="43"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C21" s="43"/>
     </row>

</xml_diff>

<commit_message>
adds profile metadata in RDF serliasations
closes #141
</commit_message>
<xml_diff>
--- a/code/vocab_csv/process.xlsx
+++ b/code/vocab_csv/process.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="304">
   <si>
     <t>preffix</t>
   </si>
@@ -447,6 +447,24 @@
   </si>
   <si>
     <t>Schema.org vocabulary</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dx/prof/</t>
+  </si>
+  <si>
+    <t>Profiles</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dx/prof/role/</t>
+  </si>
+  <si>
+    <t>Roles</t>
   </si>
   <si>
     <t>dpv-nace</t>
@@ -2552,6 +2570,28 @@
         <v>143</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -2577,8 +2617,10 @@
     <hyperlink r:id="rId21" ref="B22"/>
     <hyperlink r:id="rId22" ref="B23"/>
     <hyperlink r:id="rId23" ref="B24"/>
+    <hyperlink r:id="rId24" ref="B25"/>
+    <hyperlink r:id="rId25" ref="B26"/>
   </hyperlinks>
-  <drawing r:id="rId24"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -2594,10 +2636,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="28" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>28</v>
@@ -2614,13 +2656,13 @@
     </row>
     <row r="2">
       <c r="A2" s="30" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -2634,13 +2676,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -2654,13 +2696,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -2669,18 +2711,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -2689,34 +2731,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -2730,13 +2772,13 @@
     </row>
     <row r="8">
       <c r="A8" s="30" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -2750,13 +2792,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -2770,13 +2812,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -2785,18 +2827,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -2805,18 +2847,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -2825,18 +2867,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -2850,13 +2892,13 @@
     </row>
     <row r="14">
       <c r="A14" s="30" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -2870,13 +2912,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -2890,13 +2932,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -2905,18 +2947,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -2925,18 +2967,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -2945,18 +2987,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -2970,13 +3012,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -2990,13 +3032,13 @@
     </row>
     <row r="21">
       <c r="A21" s="31" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="D21" s="33">
         <v>44734.0</v>
@@ -3026,13 +3068,13 @@
     </row>
     <row r="22">
       <c r="A22" s="31" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="D22" s="33">
         <v>44734.0</v>
@@ -3062,13 +3104,13 @@
     </row>
     <row r="23">
       <c r="A23" s="31" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="D23" s="33">
         <v>44734.0</v>
@@ -3098,13 +3140,13 @@
     </row>
     <row r="24">
       <c r="A24" s="31" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D24" s="33">
         <v>45189.0</v>
@@ -3208,49 +3250,49 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="35" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -3270,25 +3312,25 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="8">
@@ -3298,30 +3340,30 @@
         <v>45270.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
@@ -3331,10 +3373,10 @@
       <c r="K3" s="41"/>
       <c r="L3" s="41"/>
       <c r="M3" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -3357,19 +3399,19 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
@@ -3379,10 +3421,10 @@
       <c r="K4" s="41"/>
       <c r="L4" s="41"/>
       <c r="M4" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
@@ -3405,34 +3447,34 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
       <c r="I5" s="6" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
       <c r="M5" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
@@ -3455,60 +3497,60 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
       <c r="I7" s="6" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="J7" s="41"/>
       <c r="K7" s="41"/>
       <c r="L7" s="41"/>
       <c r="M7" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="41"/>
@@ -6474,49 +6516,49 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="H1" s="47" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="I1" s="47" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
       <c r="J1" s="48" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="N1" s="50" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -6534,23 +6576,23 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E2" s="41" t="str">
         <f>CONCATENATE("dpv:",RIGHT(A2,LEN(A2) - 3))</f>
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -6561,13 +6603,13 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
@@ -6585,22 +6627,22 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -6611,10 +6653,10 @@
       </c>
       <c r="L3" s="41"/>
       <c r="M3" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -6633,22 +6675,22 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>274</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>268</v>
       </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
@@ -6659,10 +6701,10 @@
       </c>
       <c r="L4" s="41"/>
       <c r="M4" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
@@ -6681,22 +6723,22 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
@@ -6707,10 +6749,10 @@
       </c>
       <c r="L5" s="41"/>
       <c r="M5" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
@@ -6729,27 +6771,27 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
       <c r="I6" s="6" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="J6" s="41"/>
       <c r="K6" s="8">
@@ -6757,10 +6799,10 @@
       </c>
       <c r="L6" s="41"/>
       <c r="M6" s="6" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="41"/>
@@ -6779,22 +6821,22 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
@@ -6805,10 +6847,10 @@
       </c>
       <c r="L7" s="41"/>
       <c r="M7" s="6" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="41"/>
@@ -6848,43 +6890,43 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="C15" s="43"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="C16" s="43"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="C17" s="43"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="C18" s="43"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="C19" s="43"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C20" s="43"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="C21" s="43"/>
     </row>

</xml_diff>

<commit_message>
adds EU NIS2 extension (stub with Notice concepts)
- see #147 for discussion
</commit_message>
<xml_diff>
--- a/code/vocab_csv/process.xlsx
+++ b/code/vocab_csv/process.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="307">
   <si>
     <t>preffix</t>
   </si>
@@ -168,6 +168,15 @@
   </si>
   <si>
     <t>EU-AI Act concepts extended DPV</t>
+  </si>
+  <si>
+    <t>eu-nis2</t>
+  </si>
+  <si>
+    <t>https://w3id.org/dpv/legal/eu/nis2#</t>
+  </si>
+  <si>
+    <t>EU-NIS2 concepts extended DPV</t>
   </si>
   <si>
     <t>loc</t>
@@ -1856,13 +1865,13 @@
       <c r="H15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D16" s="14"/>
@@ -1874,17 +1883,17 @@
       <c r="H16" s="14"/>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="14"/>
@@ -1895,7 +1904,7 @@
       <c r="A18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C18" s="16" t="s">
@@ -1923,6 +1932,9 @@
       <c r="E19" s="16" t="s">
         <v>11</v>
       </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
@@ -1970,16 +1982,17 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="D23" s="14"/>
+      <c r="E23" s="16" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1994,6 +2007,20 @@
         <v>77</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2024,8 +2051,9 @@
     <hyperlink r:id="rId23" ref="B22"/>
     <hyperlink r:id="rId24" ref="B23"/>
     <hyperlink r:id="rId25" ref="B24"/>
+    <hyperlink r:id="rId26" ref="B25"/>
   </hyperlinks>
-  <drawing r:id="rId26"/>
+  <drawing r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -2071,13 +2099,13 @@
     </row>
     <row r="2">
       <c r="A2" s="19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
@@ -2101,13 +2129,13 @@
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
@@ -2131,13 +2159,13 @@
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
@@ -2161,13 +2189,13 @@
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -2191,13 +2219,13 @@
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
@@ -2221,13 +2249,13 @@
     </row>
     <row r="7">
       <c r="A7" s="19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -2251,10 +2279,10 @@
     </row>
     <row r="8">
       <c r="A8" s="19" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C8" s="25" t="str">
         <f>HYPERLINK("https://www.specialprivacy.eu/images/documents/SPECIAL_D25_M21_V10.pdf","SPECIAL Log vocabulary cf. SPECIAL Deliverable D2.5")</f>
@@ -2282,13 +2310,13 @@
     </row>
     <row r="9">
       <c r="A9" s="19" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -2312,13 +2340,13 @@
     </row>
     <row r="10">
       <c r="A10" s="19" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
@@ -2342,13 +2370,13 @@
     </row>
     <row r="11">
       <c r="A11" s="27" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
@@ -2372,13 +2400,13 @@
     </row>
     <row r="12">
       <c r="A12" s="19" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
@@ -2402,13 +2430,13 @@
     </row>
     <row r="13">
       <c r="A13" s="19" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
@@ -2432,13 +2460,13 @@
     </row>
     <row r="14">
       <c r="A14" s="27" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
@@ -2462,134 +2490,134 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2636,10 +2664,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="28" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>28</v>
@@ -2656,13 +2684,13 @@
     </row>
     <row r="2">
       <c r="A2" s="30" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D2" s="8">
         <v>44601.0</v>
@@ -2676,13 +2704,13 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D3" s="8">
         <v>44601.0</v>
@@ -2696,13 +2724,13 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D4" s="8">
         <v>44727.0</v>
@@ -2711,18 +2739,18 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D5" s="8">
         <v>44650.0</v>
@@ -2731,34 +2759,34 @@
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D7" s="8">
         <v>44601.0</v>
@@ -2772,13 +2800,13 @@
     </row>
     <row r="8">
       <c r="A8" s="30" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D8" s="8">
         <v>44601.0</v>
@@ -2792,13 +2820,13 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D9" s="8">
         <v>44601.0</v>
@@ -2812,13 +2840,13 @@
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="D10" s="8">
         <v>44727.0</v>
@@ -2827,18 +2855,18 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D11" s="8">
         <v>44650.0</v>
@@ -2847,18 +2875,18 @@
         <v>11</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D12" s="8">
         <v>44650.0</v>
@@ -2867,18 +2895,18 @@
         <v>11</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D13" s="8">
         <v>44601.0</v>
@@ -2892,13 +2920,13 @@
     </row>
     <row r="14">
       <c r="A14" s="30" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D14" s="8">
         <v>44601.0</v>
@@ -2912,13 +2940,13 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D15" s="8">
         <v>44601.0</v>
@@ -2932,13 +2960,13 @@
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D16" s="8">
         <v>44727.0</v>
@@ -2947,18 +2975,18 @@
         <v>11</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D17" s="8">
         <v>44650.0</v>
@@ -2967,18 +2995,18 @@
         <v>11</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D18" s="8">
         <v>44650.0</v>
@@ -2987,18 +3015,18 @@
         <v>11</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D19" s="8">
         <v>44734.0</v>
@@ -3012,13 +3040,13 @@
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D20" s="8">
         <v>44734.0</v>
@@ -3032,13 +3060,13 @@
     </row>
     <row r="21">
       <c r="A21" s="31" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D21" s="33">
         <v>44734.0</v>
@@ -3068,13 +3096,13 @@
     </row>
     <row r="22">
       <c r="A22" s="31" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D22" s="33">
         <v>44734.0</v>
@@ -3104,13 +3132,13 @@
     </row>
     <row r="23">
       <c r="A23" s="31" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D23" s="33">
         <v>44734.0</v>
@@ -3140,13 +3168,13 @@
     </row>
     <row r="24">
       <c r="A24" s="31" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D24" s="33">
         <v>45189.0</v>
@@ -3250,49 +3278,49 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="35" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F1" s="35" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K1" s="37" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="L1" s="37" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -3312,25 +3340,25 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="8">
@@ -3340,30 +3368,30 @@
         <v>45270.0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
@@ -3373,10 +3401,10 @@
       <c r="K3" s="41"/>
       <c r="L3" s="41"/>
       <c r="M3" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -3399,19 +3427,19 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F4" s="41"/>
       <c r="G4" s="41"/>
@@ -3421,10 +3449,10 @@
       <c r="K4" s="41"/>
       <c r="L4" s="41"/>
       <c r="M4" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
@@ -3447,34 +3475,34 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
       <c r="I5" s="6" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
       <c r="L5" s="41"/>
       <c r="M5" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
@@ -3497,60 +3525,60 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F7" s="41"/>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
       <c r="I7" s="6" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="J7" s="41"/>
       <c r="K7" s="41"/>
       <c r="L7" s="41"/>
       <c r="M7" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="41"/>
@@ -6516,49 +6544,49 @@
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="G1" s="47" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H1" s="47" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="I1" s="47" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="J1" s="48" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K1" s="49" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="L1" s="49" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="N1" s="50" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
@@ -6576,23 +6604,23 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E2" s="41" t="str">
         <f>CONCATENATE("dpv:",RIGHT(A2,LEN(A2) - 3))</f>
         <v>dpv:PersonalDataHandling</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -6603,13 +6631,13 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
@@ -6627,22 +6655,22 @@
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>277</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>279</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>274</v>
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -6653,10 +6681,10 @@
       </c>
       <c r="L3" s="41"/>
       <c r="M3" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
@@ -6675,22 +6703,22 @@
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
@@ -6701,10 +6729,10 @@
       </c>
       <c r="L4" s="41"/>
       <c r="M4" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
@@ -6723,22 +6751,22 @@
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G5" s="41"/>
       <c r="H5" s="41"/>
@@ -6749,10 +6777,10 @@
       </c>
       <c r="L5" s="41"/>
       <c r="M5" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O5" s="41"/>
       <c r="P5" s="41"/>
@@ -6771,27 +6799,27 @@
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
       <c r="I6" s="6" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="J6" s="41"/>
       <c r="K6" s="8">
@@ -6799,10 +6827,10 @@
       </c>
       <c r="L6" s="41"/>
       <c r="M6" s="6" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O6" s="41"/>
       <c r="P6" s="41"/>
@@ -6821,22 +6849,22 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
@@ -6847,10 +6875,10 @@
       </c>
       <c r="L7" s="41"/>
       <c r="M7" s="6" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="O7" s="41"/>
       <c r="P7" s="41"/>
@@ -6890,43 +6918,43 @@
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C15" s="43"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C16" s="43"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C17" s="43"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C18" s="43"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C19" s="43"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C20" s="43"/>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C21" s="43"/>
     </row>

</xml_diff>